<commit_message>
adding copy until max feature
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitrepos\github\crgarcia12\powershell-excelinteraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5932DE60-3C13-4D9A-87C0-6F2A93091CC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E7049F-73D5-4FDA-9210-5CA1765DE399}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2990" yWindow="2120" windowWidth="19200" windowHeight="10060" activeTab="1" xr2:uid="{F94279EE-5BD5-45DA-AE9D-B3C67DC4CD85}"/>
+    <workbookView xWindow="5320" yWindow="5930" windowWidth="19200" windowHeight="10060" xr2:uid="{F94279EE-5BD5-45DA-AE9D-B3C67DC4CD85}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECDD676-FB1A-4F85-85E5-66F1F51C3280}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,13 +425,13 @@
         <v>0.5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -440,13 +440,13 @@
         <v>0.50001157407407404</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -455,13 +455,13 @@
         <v>0.50002314814814797</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -470,13 +470,13 @@
         <v>0.50003472222222201</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -485,13 +485,13 @@
         <v>0.50004629629629604</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -500,13 +500,13 @@
         <v>0.50005787037036997</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -515,13 +515,13 @@
         <v>0.50006944444444401</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -530,13 +530,13 @@
         <v>0.50008101851851805</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -545,13 +545,13 @@
         <v>0.50009259259259198</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -560,30 +560,15 @@
         <v>0.50010416666666602</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>0.50011574074073994</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>30</v>
-      </c>
-      <c r="D12">
-        <v>50</v>
-      </c>
-      <c r="I12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -596,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{834E9E7F-B525-4D39-8BD2-4B9F7DC1D423}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>